<commit_message>
NhanVo: Update MySQL docker
</commit_message>
<xml_diff>
--- a/BridgeNetwork/GuideLine.xlsx
+++ b/BridgeNetwork/GuideLine.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>GIT: https://github.com/nhanvo/alpine-apache-php.git</t>
   </si>
@@ -82,9 +82,6 @@
     <t>docker inspect alpine-apache-php</t>
   </si>
   <si>
-    <t>4.5 Disconnect network</t>
-  </si>
-  <si>
     <t>docker network disconnect bridge alpine-apache-php</t>
   </si>
   <si>
@@ -92,6 +89,48 @@
   </si>
   <si>
     <t>Link: http://localhost:8080/master.php</t>
+  </si>
+  <si>
+    <t>GIT: https://github.com/container-examples/alpine-mysql.git</t>
+  </si>
+  <si>
+    <t>1. Checkout alpine mysql</t>
+  </si>
+  <si>
+    <t>2. Build images from source</t>
+  </si>
+  <si>
+    <t>docker build -t alpine-mysql:latest .</t>
+  </si>
+  <si>
+    <t>3. Check images build successful</t>
+  </si>
+  <si>
+    <t>docker images</t>
+  </si>
+  <si>
+    <t>4. Build containers</t>
+  </si>
+  <si>
+    <t>docker run -d --name alpine-mysql -p 3306:3306 --env-file .env alpine-mysql</t>
+  </si>
+  <si>
+    <t>5. Set network for mysql container</t>
+  </si>
+  <si>
+    <t>docker inspect alpine-mysql</t>
+  </si>
+  <si>
+    <t>docker network connect www-net alpine-mysql</t>
+  </si>
+  <si>
+    <t>docker network disconnect bridge alpine-mysql</t>
+  </si>
+  <si>
+    <t>4.5 Disconnect bridge default network</t>
+  </si>
+  <si>
+    <t>6. Disconnect bridge default network</t>
   </si>
 </sst>
 </file>
@@ -2243,6 +2282,799 @@
         <a:xfrm>
           <a:off x="11547763" y="41854582"/>
           <a:ext cx="1593273" cy="277092"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>265353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>13858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="9485553"/>
+          <a:ext cx="10058400" cy="2542505"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="863600" y="1117600"/>
+          <a:ext cx="4940300" cy="3302000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1193800" y="2374901"/>
+          <a:ext cx="1943100" cy="1968499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>203201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1155700" y="10820401"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>10386</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="5588000"/>
+          <a:ext cx="10058400" cy="2804386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>266701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5181600" y="6413501"/>
+          <a:ext cx="3898900" cy="330199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9569</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>19711</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847769" y="13131800"/>
+          <a:ext cx="11186142" cy="1854200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="13728701"/>
+          <a:ext cx="5346700" cy="241299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2387600" y="14325601"/>
+          <a:ext cx="1041400" cy="215899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="16205200"/>
+          <a:ext cx="8826500" cy="3759200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5232400" y="17322800"/>
+          <a:ext cx="2984500" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10337800" y="16205200"/>
+          <a:ext cx="4025900" cy="3873500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10579100" y="16205200"/>
+          <a:ext cx="939800" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="20955000"/>
+          <a:ext cx="4508500" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="21196300"/>
+          <a:ext cx="3505200" cy="3937000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2629,8 +3461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AK2:AM150"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ126" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="CK147" sqref="CK147"/>
+    <sheetView topLeftCell="AJ105" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="AL120" sqref="AL120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2692,22 +3524,22 @@
     </row>
     <row r="120" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AL120" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM121" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AM121" s="1" t="s">
+    <row r="149" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AL149" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL149" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="150" spans="38:39" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AM150" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2719,10 +3551,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+  <dimension ref="B2:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="AK82" sqref="AK82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2730,12 +3562,73 @@
     <col min="2" max="2" width="3.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3">
-        <v>1</v>
+    <row r="2" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NhanVo: Finish setup Apache, PHP, MySQL
</commit_message>
<xml_diff>
--- a/BridgeNetwork/GuideLine.xlsx
+++ b/BridgeNetwork/GuideLine.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Create Bridge Network" sheetId="2" r:id="rId1"/>
     <sheet name="Apache_PHP" sheetId="1" r:id="rId2"/>
     <sheet name="MySQL" sheetId="3" r:id="rId3"/>
+    <sheet name="Normal error" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -2039,8 +2040,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16279090" y="28390272"/>
-          <a:ext cx="1743365" cy="496455"/>
+          <a:off x="15992103" y="27885570"/>
+          <a:ext cx="1708729" cy="486559"/>
           <a:chOff x="16279090" y="28390272"/>
           <a:chExt cx="1743365" cy="496455"/>
         </a:xfrm>
@@ -3381,8 +3382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AN51"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="AN51" sqref="AN51"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3461,7 +3462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AK2:AM150"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ105" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AL120" sqref="AL120"/>
     </sheetView>
   </sheetViews>
@@ -3553,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="AK82" sqref="AK82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3631,4 +3632,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>